<commit_message>
Master sql for db creation
</commit_message>
<xml_diff>
--- a/DBMentorshipPlatformBPIT.xlsx
+++ b/DBMentorshipPlatformBPIT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t xml:space="preserve">userId </t>
   </si>
@@ -90,27 +90,18 @@
     <t>libraryId</t>
   </si>
   <si>
-    <t>nameOfUploadedFile</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
     <t>varchar(20)</t>
   </si>
   <si>
-    <t>category</t>
-  </si>
-  <si>
     <t>varchar(30)</t>
   </si>
   <si>
     <t>locationOfUploadedFile</t>
   </si>
   <si>
-    <t>varchar(300)</t>
-  </si>
-  <si>
     <t>uploadDate</t>
   </si>
   <si>
@@ -142,6 +133,18 @@
   </si>
   <si>
     <t>Physics | Chem | ..... | Accounts etc</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+  </si>
+  <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>stream</t>
   </si>
 </sst>
 </file>
@@ -269,9 +272,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -283,6 +283,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -593,16 +596,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="25.8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -662,39 +665,39 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="25.8">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="10"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -707,30 +710,30 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="25.8">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
@@ -738,79 +741,87 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="25.8">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="10"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="25.8" customHeight="1">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -818,7 +829,7 @@
     <row r="32" spans="1:3" ht="14.4" customHeight="1"/>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>